<commit_message>
Selenium 21. gün JsExacutor
</commit_message>
<xml_diff>
--- a/src/test/java/techproed/resources/Capitals.xlsx
+++ b/src/test/java/techproed/resources/Capitals.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\OneDrive\Masaüstü\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TechProEducation\B151MavenJUnit\src\test\java\techproed\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>COUNTRY</t>
   </si>
@@ -85,12 +85,22 @@
   </si>
   <si>
     <t>Oslo</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>Pekin</t>
+  </si>
+  <si>
+    <t>NUFUS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -352,55 +362,70 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" t="s" s="0">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" t="n" s="0">
+        <v>712816.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C3" t="n" s="0">
+        <v>2161000.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C4" t="n" s="0">
+        <v>8982000.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" t="n" s="0">
+        <v>5663000.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
@@ -408,7 +433,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
@@ -416,7 +441,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -424,7 +449,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -432,7 +457,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -440,12 +465,20 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>